<commit_message>
Argh - fix .Rnw after crash
</commit_message>
<xml_diff>
--- a/R/raw_data/source_data/PSE-Database_Study_level_descriptives.xlsx
+++ b/R/raw_data/source_data/PSE-Database_Study_level_descriptives.xlsx
@@ -80,184 +80,184 @@
     <t xml:space="preserve">2014-2015</t>
   </si>
   <si>
+    <t xml:space="preserve">DE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">i</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mostly students</t>
+  </si>
+  <si>
+    <t xml:space="preserve">yes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CZ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Munich</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2013</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">students</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FS_ErlSem</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2015</t>
+  </si>
+  <si>
+    <t xml:space="preserve">H</t>
+  </si>
+  <si>
+    <t xml:space="preserve">g</t>
+  </si>
+  <si>
+    <t xml:space="preserve">no</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FS_MOCO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mostly non-students</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FS_newpic</t>
+  </si>
+  <si>
+    <t xml:space="preserve">variable</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2016</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FS_TSST</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2nd_sentence_rule</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2011-2012</t>
+  </si>
+  <si>
+    <t xml:space="preserve">JP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2016-2018</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CL &amp; CO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KJ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Erlangen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-2019</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MK1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">N/A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MK2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MK3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MOJ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MQ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2012</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OCS_Bp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OCS_smofee6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2010</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OCS_smofee7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OCS_smofee8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OCS_smofee9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PMK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2016-2017</t>
+  </si>
+  <si>
+    <t xml:space="preserve">students and non-students</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RMH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TC_SNF6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Trier</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TC_SNF7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TC_TAI1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Timestamp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Untitled Question</t>
+  </si>
+  <si>
+    <t xml:space="preserve">de (Osnabrück)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">de (Munich)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">de (Erlangen)</t>
+  </si>
+  <si>
     <t xml:space="preserve">de</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">i</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mostly students</t>
-  </si>
-  <si>
-    <t xml:space="preserve">yes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CZ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Munich</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2013</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">students</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FS_ErlSem</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2015</t>
-  </si>
-  <si>
-    <t xml:space="preserve">H</t>
-  </si>
-  <si>
-    <t xml:space="preserve">g</t>
-  </si>
-  <si>
-    <t xml:space="preserve">no</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FS_MOCO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mostly non-students</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FS_newpic</t>
-  </si>
-  <si>
-    <t xml:space="preserve">variable</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2016</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FS_TSST</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2nd_sentence_rule</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2011-2012</t>
-  </si>
-  <si>
-    <t xml:space="preserve">JP</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2016-2018</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CL &amp; CO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">KJ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Erlangen</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LI</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2018-2019</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MK1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">N/A</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MK2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MK3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MOJ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MQ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2012</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NK</t>
-  </si>
-  <si>
-    <t xml:space="preserve">OCS_Bp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">OCS_smofee6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2010</t>
-  </si>
-  <si>
-    <t xml:space="preserve">OCS_smofee7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">OCS_smofee8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">OCS_smofee9</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PMK</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2016-2017</t>
-  </si>
-  <si>
-    <t xml:space="preserve">students and non-students</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RMH</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TC_SNF6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Trier</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CH</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TC_SNF7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TC_TAI1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Timestamp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Untitled Question</t>
-  </si>
-  <si>
-    <t xml:space="preserve">de (Osnabrück)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">de (Munich)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">de (Erlangen)</t>
   </si>
   <si>
     <t xml:space="preserve">de (Göttingen)</t>
@@ -492,11 +492,11 @@
   <dimension ref="A1:Z27"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="F8" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="F1" activeCellId="0" sqref="F1"/>
-      <selection pane="bottomLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
-      <selection pane="bottomRight" activeCell="I31" activeCellId="0" sqref="I31"/>
+      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="I6" activeCellId="0" sqref="I2:I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -847,10 +847,10 @@
         <v>43</v>
       </c>
       <c r="I8" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="J8" s="6" t="s">
         <v>44</v>
-      </c>
-      <c r="J8" s="6" t="s">
-        <v>45</v>
       </c>
       <c r="K8" s="6" t="s">
         <v>21</v>
@@ -865,7 +865,7 @@
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B9" s="4" t="n">
         <v>671</v>
@@ -880,7 +880,7 @@
         <v>15</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G9" s="4" t="s">
         <v>37</v>
@@ -889,7 +889,7 @@
         <v>30</v>
       </c>
       <c r="I9" s="6" t="s">
-        <v>44</v>
+        <v>19</v>
       </c>
       <c r="J9" s="6" t="s">
         <v>20</v>
@@ -907,7 +907,7 @@
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B10" s="4"/>
       <c r="C10" s="4"/>
@@ -924,10 +924,10 @@
         <v>17</v>
       </c>
       <c r="H10" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="I10" s="6" t="s">
-        <v>44</v>
+        <v>19</v>
       </c>
       <c r="J10" s="8" t="s">
         <v>27</v>
@@ -945,7 +945,7 @@
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B11" s="4" t="n">
         <v>804</v>
@@ -960,7 +960,7 @@
         <v>15</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G11" s="4" t="s">
         <v>37</v>
@@ -969,7 +969,7 @@
         <v>30</v>
       </c>
       <c r="I11" s="6" t="s">
-        <v>44</v>
+        <v>19</v>
       </c>
       <c r="J11" s="6" t="s">
         <v>20</v>
@@ -978,7 +978,7 @@
         <v>21</v>
       </c>
       <c r="L11" s="6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="M11" s="7"/>
       <c r="N11" s="4" t="s">
@@ -987,7 +987,7 @@
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B12" s="4" t="n">
         <v>600</v>
@@ -1002,7 +1002,7 @@
         <v>15</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G12" s="4" t="s">
         <v>37</v>
@@ -1011,7 +1011,7 @@
         <v>26</v>
       </c>
       <c r="I12" s="6" t="s">
-        <v>44</v>
+        <v>19</v>
       </c>
       <c r="J12" s="6" t="s">
         <v>20</v>
@@ -1020,7 +1020,7 @@
         <v>21</v>
       </c>
       <c r="L12" s="6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="M12" s="7"/>
       <c r="N12" s="4" t="s">
@@ -1029,7 +1029,7 @@
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B13" s="4" t="n">
         <v>773</v>
@@ -1044,7 +1044,7 @@
         <v>15</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G13" s="4" t="s">
         <v>37</v>
@@ -1053,7 +1053,7 @@
         <v>30</v>
       </c>
       <c r="I13" s="6" t="s">
-        <v>44</v>
+        <v>19</v>
       </c>
       <c r="J13" s="6" t="s">
         <v>20</v>
@@ -1062,7 +1062,7 @@
         <v>21</v>
       </c>
       <c r="L13" s="6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="M13" s="7"/>
       <c r="N13" s="4" t="s">
@@ -1071,7 +1071,7 @@
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B14" s="4" t="n">
         <v>149</v>
@@ -1095,7 +1095,7 @@
         <v>38</v>
       </c>
       <c r="I14" s="6" t="s">
-        <v>44</v>
+        <v>19</v>
       </c>
       <c r="J14" s="6" t="s">
         <v>20</v>
@@ -1115,7 +1115,7 @@
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B15" s="4" t="n">
         <v>486</v>
@@ -1136,10 +1136,10 @@
         <v>17</v>
       </c>
       <c r="H15" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="I15" s="6" t="s">
-        <v>44</v>
+        <v>19</v>
       </c>
       <c r="J15" s="8" t="s">
         <v>27</v>
@@ -1157,7 +1157,7 @@
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B16" s="4" t="n">
         <v>825</v>
@@ -1181,7 +1181,7 @@
         <v>30</v>
       </c>
       <c r="I16" s="6" t="s">
-        <v>44</v>
+        <v>19</v>
       </c>
       <c r="J16" s="8" t="s">
         <v>27</v>
@@ -1199,7 +1199,7 @@
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B17" s="4" t="n">
         <v>653</v>
@@ -1214,7 +1214,7 @@
         <v>15</v>
       </c>
       <c r="F17" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G17" s="4" t="s">
         <v>37</v>
@@ -1223,7 +1223,7 @@
         <v>26</v>
       </c>
       <c r="I17" s="6" t="s">
-        <v>44</v>
+        <v>19</v>
       </c>
       <c r="J17" s="6" t="s">
         <v>20</v>
@@ -1243,7 +1243,7 @@
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B18" s="4" t="n">
         <v>984</v>
@@ -1258,16 +1258,16 @@
         <v>40</v>
       </c>
       <c r="F18" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G18" s="4" t="s">
         <v>37</v>
       </c>
       <c r="H18" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="I18" s="6" t="s">
-        <v>44</v>
+        <v>19</v>
       </c>
       <c r="J18" s="6" t="s">
         <v>20</v>
@@ -1287,7 +1287,7 @@
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B19" s="4" t="n">
         <v>930</v>
@@ -1302,7 +1302,7 @@
         <v>40</v>
       </c>
       <c r="F19" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G19" s="4" t="s">
         <v>37</v>
@@ -1311,7 +1311,7 @@
         <v>41</v>
       </c>
       <c r="I19" s="6" t="s">
-        <v>44</v>
+        <v>19</v>
       </c>
       <c r="J19" s="6" t="s">
         <v>20</v>
@@ -1331,7 +1331,7 @@
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B20" s="4" t="n">
         <v>888</v>
@@ -1346,16 +1346,16 @@
         <v>15</v>
       </c>
       <c r="F20" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G20" s="4" t="s">
         <v>37</v>
       </c>
       <c r="H20" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="I20" s="6" t="s">
-        <v>44</v>
+        <v>19</v>
       </c>
       <c r="J20" s="6" t="s">
         <v>20</v>
@@ -1375,7 +1375,7 @@
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B21" s="4" t="n">
         <v>893</v>
@@ -1390,16 +1390,16 @@
         <v>40</v>
       </c>
       <c r="F21" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G21" s="4" t="s">
         <v>37</v>
       </c>
       <c r="H21" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="I21" s="6" t="s">
-        <v>44</v>
+        <v>19</v>
       </c>
       <c r="J21" s="6" t="s">
         <v>20</v>
@@ -1419,7 +1419,7 @@
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B22" s="4" t="n">
         <v>1772</v>
@@ -1440,10 +1440,10 @@
         <v>17</v>
       </c>
       <c r="H22" s="5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="I22" s="6" t="s">
-        <v>44</v>
+        <v>19</v>
       </c>
       <c r="J22" s="8" t="s">
         <v>27</v>
@@ -1452,7 +1452,7 @@
         <v>21</v>
       </c>
       <c r="L22" s="6" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="M22" s="6"/>
       <c r="N22" s="4" t="s">
@@ -1461,7 +1461,7 @@
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B23" s="4" t="n">
         <v>698</v>
@@ -1485,7 +1485,7 @@
         <v>38</v>
       </c>
       <c r="I23" s="6" t="s">
-        <v>44</v>
+        <v>19</v>
       </c>
       <c r="J23" s="6" t="s">
         <v>20</v>
@@ -1503,7 +1503,7 @@
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B24" s="4" t="n">
         <v>676</v>
@@ -1518,7 +1518,7 @@
         <v>40</v>
       </c>
       <c r="F24" s="4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G24" s="4" t="s">
         <v>17</v>
@@ -1527,7 +1527,7 @@
         <v>30</v>
       </c>
       <c r="I24" s="6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="J24" s="8" t="s">
         <v>27</v>
@@ -1545,7 +1545,7 @@
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B25" s="4" t="n">
         <v>1211</v>
@@ -1560,7 +1560,7 @@
         <v>40</v>
       </c>
       <c r="F25" s="4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G25" s="4" t="s">
         <v>17</v>
@@ -1569,7 +1569,7 @@
         <v>38</v>
       </c>
       <c r="I25" s="6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="J25" s="8" t="s">
         <v>27</v>
@@ -1587,7 +1587,7 @@
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B26" s="4" t="n">
         <v>981</v>
@@ -1602,7 +1602,7 @@
         <v>40</v>
       </c>
       <c r="F26" s="4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G26" s="4" t="s">
         <v>17</v>
@@ -1611,7 +1611,7 @@
         <v>30</v>
       </c>
       <c r="I26" s="6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="J26" s="8" t="s">
         <v>27</v>
@@ -1629,7 +1629,7 @@
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D27" s="4" t="n">
         <v>6</v>
@@ -1644,10 +1644,10 @@
         <v>17</v>
       </c>
       <c r="H27" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="I27" s="6" t="s">
-        <v>44</v>
+        <v>19</v>
       </c>
       <c r="J27" s="8" t="s">
         <v>27</v>
@@ -1656,7 +1656,7 @@
         <v>21</v>
       </c>
       <c r="L27" s="6" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="M27" s="7"/>
       <c r="N27" s="0" t="s">
@@ -1684,7 +1684,7 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="A2" activeCellId="1" sqref="I2:I6 A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1695,40 +1695,40 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="B1" s="4" t="s">
         <v>74</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="6" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="6" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="6" t="s">
-        <v>19</v>
+        <v>78</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="6" t="s">
-        <v>19</v>
+        <v>78</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1738,77 +1738,77 @@
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="6" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="10" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="6" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="6" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="6" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="6" t="s">
-        <v>19</v>
+        <v>78</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="6" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="6" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="6" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="6" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="6" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="6" t="s">
-        <v>19</v>
+        <v>78</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1828,7 +1828,7 @@
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="6" t="s">
-        <v>19</v>
+        <v>78</v>
       </c>
     </row>
   </sheetData>

</xml_diff>